<commit_message>
Mejoras en la aplicación embebida
1.- Mejoras en el sistema de posicionamiento del equipo de riego.
</commit_message>
<xml_diff>
--- a/Calibración de equipos.xlsx
+++ b/Calibración de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB34776-0446-4552-ADA5-CF7625A438BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4485E7-5478-4A2E-8C43-4366FB598A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="484" activeTab="2" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="484" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Equipo</t>
-  </si>
-  <si>
-    <t>Calibración</t>
   </si>
   <si>
     <t>Software</t>
@@ -59,33 +56,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>(-937, 515, -962, 653, -1033, 0)</t>
-  </si>
-  <si>
-    <t>(-607, 910, -950, 888, -1140, 0)</t>
-  </si>
-  <si>
-    <t>(-653, 1005, -890, 698, -1320, 0)</t>
-  </si>
-  <si>
-    <t>(-568, 952, -813, 866, -1290, 0)</t>
-  </si>
-  <si>
-    <t>(-810, 935, -1112, 685, -1267, 0)</t>
-  </si>
-  <si>
-    <t>(-665, 947, -663, 776, -1426, 0)</t>
-  </si>
-  <si>
-    <t>(-760, 1030, -1003, 685, -1366, 0)</t>
-  </si>
-  <si>
-    <t>(-820, 890, -782, 1065, -1248, 0)</t>
-  </si>
-  <si>
-    <t>(-527, 1083, -291, 908, -1595, 0)</t>
-  </si>
-  <si>
     <t>Servidor</t>
   </si>
   <si>
@@ -93,15 +63,6 @@
   </si>
   <si>
     <t>Observaciones</t>
-  </si>
-  <si>
-    <t>(-706, 1043, -1268, 806, -1433, 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicona | </t>
-  </si>
-  <si>
-    <t>(-838, 622, -892, 702, -792, 0)</t>
   </si>
   <si>
     <t>JQC - 1</t>
@@ -119,58 +80,13 @@
     <t>Johan</t>
   </si>
   <si>
-    <t>(-801, 622, -986, 557, -762, 17)</t>
-  </si>
-  <si>
     <t>FL - 0</t>
-  </si>
-  <si>
-    <t>(-467, 752, -638, 866, -1102, 0)</t>
-  </si>
-  <si>
-    <t>Claudio</t>
-  </si>
-  <si>
-    <t>Pv66 v0.2.3 R</t>
-  </si>
-  <si>
-    <t>Silicona | Actualizado | Ok</t>
-  </si>
-  <si>
-    <t>Silicona | Problema presión</t>
-  </si>
-  <si>
-    <t>(-1020, 585, -752, 827, -1376, 0)</t>
   </si>
   <si>
     <t>Aux</t>
   </si>
   <si>
-    <t>(-337, 1230, 0, 2471, -1653, 0)</t>
-  </si>
-  <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>(-610, 840, 0, 2155, -2382, 0)</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
     <t>grados</t>
-  </si>
-  <si>
-    <t>(-672, 741, 0, 1878, 0, 176)</t>
-  </si>
-  <si>
-    <t>(-350, 1278, 0, 2030, -91, 32)</t>
-  </si>
-  <si>
-    <t>(-450, 1056, 0, 1901, 0, 227)</t>
-  </si>
-  <si>
-    <t>(-452, 1110, 0, 2002, 0, 336)</t>
   </si>
   <si>
     <t>(-511, 1017, 0, 2027, 0, 315)</t>
@@ -228,6 +144,15 @@
   </si>
   <si>
     <t>Centro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualizado </t>
+  </si>
+  <si>
+    <t>http://pprsar.com/cosme/comm_v2.php</t>
+  </si>
+  <si>
+    <t>Pv66 v0.2.4 A</t>
   </si>
 </sst>
 </file>
@@ -2197,61 +2122,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B346EED-BC4A-47AA-A4A2-5D41F541E256}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2259,23 +2177,20 @@
         <v>526251024489</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2283,23 +2198,20 @@
         <v>526251579804</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2307,47 +2219,38 @@
         <v>526251259145</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2355,31 +2258,20 @@
         <v>526255917395</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s">
         <v>38</v>
       </c>
-      <c r="O6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2387,23 +2279,20 @@
         <v>526251193016</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2411,23 +2300,17 @@
         <v>526251201079</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2435,23 +2318,20 @@
         <v>526251452797</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2459,23 +2339,20 @@
         <v>526251060168</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2483,34 +2360,20 @@
         <v>526258372598</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2518,28 +2381,21 @@
         <v>526251271378</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2547,32 +2403,27 @@
         <v>526251531996</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2580,19 +2431,16 @@
         <v>526251342314</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2600,19 +2448,16 @@
         <v>526251037317</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2620,16 +2465,13 @@
         <v>526251059200</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2653,10 +2495,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,7 +2807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD9714C-9300-404D-9EB9-51F98C766C49}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -2980,27 +2822,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B2" s="8">
         <v>900000000</v>
@@ -3009,18 +2851,18 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>282426268</v>
@@ -3033,15 +2875,15 @@
         <v>59.894818768308966</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>282428337</v>
@@ -3064,7 +2906,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>282430372</v>
@@ -3087,7 +2929,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>282427859</v>
@@ -3110,7 +2952,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>282426805</v>
@@ -3133,7 +2975,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>282424102</v>
@@ -3156,7 +2998,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>282422085</v>
@@ -3179,7 +3021,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>282424072</v>
@@ -3202,7 +3044,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>282425926</v>
@@ -3278,13 +3120,13 @@
     <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3297,13 +3139,13 @@
         <v>127.85362853486268</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F16" s="18">
         <f>E6</f>
@@ -3318,13 +3160,13 @@
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3382,27 +3224,27 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B2" s="8">
         <v>90000000</v>
@@ -3411,13 +3253,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="G2" s="8">
         <v>90000000</v>
@@ -3428,7 +3270,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>28407276</v>
@@ -3441,10 +3283,10 @@
         <v>60.042214043738497</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="G3">
         <f>INT(INT(B3/1000000)*1000000+INT((B3/1000000-INT(B3/1000000))*60)*10000+((B3/1000000-INT(B3/1000000))*60-INT((B3/1000000-INT(B3/1000000))*60))*6000)*10</f>
@@ -3460,7 +3302,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9">
         <f>ATAN(ABS(C4 - C$3) / ABS(B4 - B$3)) * 180 / PI( )</f>
@@ -3491,7 +3333,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9">
         <f>ATAN(ABS(C5 - C$3) / ABS(B5 - B$3)) * 180 / PI( )</f>
@@ -3522,7 +3364,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>28407644</v>
@@ -3564,7 +3406,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="4"/>
@@ -3595,7 +3437,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="4"/>
@@ -3626,7 +3468,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="4"/>
@@ -3657,7 +3499,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>28406671</v>
@@ -3699,7 +3541,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>28407175</v>
@@ -3814,13 +3656,13 @@
     <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3833,13 +3675,13 @@
         <v>345.11346853390057</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F16" s="18">
         <f>E6</f>
@@ -3854,13 +3696,13 @@
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3915,24 +3757,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B2" s="8">
         <v>90</v>
@@ -3941,15 +3783,15 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B3" s="19">
         <v>28.422075</v>
@@ -3962,7 +3804,7 @@
         <v>29.802309777001746</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trabajo en sistemas J0008-1
Pv66 v0.2.4 A:
- Se eliminaron rutinas innecesarias
J0008-1 v0.2 A:
- Se ajustó el sistema para el trabajo en tiempo real
- Permite el trabajo hasta con 7 válvulas
- Se sustituyó el sistema de comunicaciones y se compatibilizó con el del Pv66 v0.2.4 A
</commit_message>
<xml_diff>
--- a/Calibración de equipos.xlsx
+++ b/Calibración de equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4485E7-5478-4A2E-8C43-4366FB598A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014BAE4-81E8-4AF4-A1CF-CFF5995D33D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="484" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="42">
   <si>
     <t>Equipo</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>Pv66 v0.2.4 A</t>
+  </si>
+  <si>
+    <t>Actualizado *</t>
+  </si>
+  <si>
+    <t>Conexión lenta al GPS</t>
+  </si>
+  <si>
+    <t>Modificar interruptor de encendido</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2137,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2196,7 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,7 +2217,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2229,7 +2238,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2268,7 +2277,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2289,7 +2298,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2328,7 +2337,7 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2349,7 +2358,10 @@
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2391,7 +2403,10 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
       </c>
       <c r="I12" s="6"/>
     </row>
@@ -2413,7 +2428,7 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mejoras en la PWA
-> Mejoras en el manejo de los sistemas de riego estacionarios
   ~ Agregar el mapeo de múltiples polígonos
   ~ Agregar la programación de los polígonos en cuanto a días | horas | minutos
   ~ Ajustes en la opción de agregar nuevo dispositivo para incluir los estacionarios
-> Cambios en la forma de mostrar los históricos de cada equipo
   ~ Se agregó iconografía
   ~ Se agregó colores en base a si estaba: Encendido / Apagado
-> Cambio de posición del Encendido y la Dirección
   ~ Vista móbil
   ~ Vista escritorio
</commit_message>
<xml_diff>
--- a/Calibración de equipos.xlsx
+++ b/Calibración de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014BAE4-81E8-4AF4-A1CF-CFF5995D33D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15C224D-D46E-4DFD-A731-73F05229C20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="484" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="484" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -2137,25 +2139,25 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2178,7 +2180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2220,7 +2222,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2259,7 +2261,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2280,7 +2282,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2319,7 +2321,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2410,7 +2412,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2431,14 +2433,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2455,7 +2457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2502,13 +2504,13 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2524,7 +2526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>20</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>60</v>
       </c>
@@ -2572,7 +2574,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>70</v>
       </c>
@@ -2580,7 +2582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>80</v>
       </c>
@@ -2588,7 +2590,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>90</v>
       </c>
@@ -2596,7 +2598,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>100</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>110</v>
       </c>
@@ -2612,7 +2614,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>120</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>130</v>
       </c>
@@ -2628,7 +2630,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>140</v>
       </c>
@@ -2636,7 +2638,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>150</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>170</v>
       </c>
@@ -2660,7 +2662,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>180</v>
       </c>
@@ -2668,7 +2670,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>190</v>
       </c>
@@ -2676,7 +2678,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>200</v>
       </c>
@@ -2684,7 +2686,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>210</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>220</v>
       </c>
@@ -2700,7 +2702,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>230</v>
       </c>
@@ -2708,7 +2710,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>240</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>250</v>
       </c>
@@ -2724,7 +2726,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>260</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>270</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>280</v>
       </c>
@@ -2748,7 +2750,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>290</v>
       </c>
@@ -2756,7 +2758,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>300</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>310</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>320</v>
       </c>
@@ -2780,7 +2782,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>330</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>340</v>
       </c>
@@ -2796,7 +2798,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>350</v>
       </c>
@@ -2804,7 +2806,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>360</v>
       </c>
@@ -2826,16 +2828,16 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -2855,7 +2857,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
@@ -2875,7 +2877,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -2919,7 +2921,7 @@
         <v>345.65371190683862</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
@@ -2988,7 +2990,7 @@
         <v>24.361651550915141</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>67.958809766553713</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -3034,7 +3036,7 @@
         <v>105.9883938172799</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
@@ -3057,7 +3059,7 @@
         <v>161.06125720466682</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3082,7 @@
         <v>205.56089781590984</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -3100,7 +3102,7 @@
         <v>195.25884947744478</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <f>F7</f>
         <v>24.361651550915141</v>
@@ -3116,7 +3118,7 @@
         <v>299.10009522643691</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <f>E7</f>
         <v>84.256470319224107</v>
@@ -3132,7 +3134,7 @@
         <v>358.99491399474584</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>24</v>
@@ -3144,7 +3146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f>F8</f>
         <v>67.958809766553713</v>
@@ -3171,7 +3173,7 @@
         <v>243.3192539009892</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -3184,7 +3186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <f>E9</f>
         <v>165.88321258558886</v>
@@ -3199,7 +3201,7 @@
         <v>265.45571658421881</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <f>F9</f>
         <v>105.9883938172799</v>
@@ -3227,17 +3229,17 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -3257,7 +3259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
@@ -3283,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -3315,7 +3317,7 @@
         <v>79.75958657020071</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -3346,7 +3348,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -3377,7 +3379,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
@@ -3419,7 +3421,7 @@
         <v>311.55235069652736</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
@@ -3450,7 +3452,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -3481,7 +3483,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -3512,7 +3514,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
@@ -3554,7 +3556,7 @@
         <v>279.68743150639153</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -3596,7 +3598,7 @@
         <v>275.34248147520822</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>28407180</v>
       </c>
@@ -3636,7 +3638,7 @@
         <v>100.24537818567508</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <f>F7</f>
         <v>285.07125449016206</v>
@@ -3652,7 +3654,7 @@
         <v>285.07125449016206</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <f>E7</f>
         <v>345.11346853390057</v>
@@ -3668,7 +3670,7 @@
         <v>345.11346853390057</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>24</v>
@@ -3680,7 +3682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f>F8</f>
         <v>285.07125449016206</v>
@@ -3707,7 +3709,7 @@
         <v>331.35274803111065</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="16"/>
       <c r="C17" s="10" t="s">
@@ -3720,7 +3722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <f>E9</f>
         <v>345.11346853390057</v>
@@ -3735,7 +3737,7 @@
         <v>355.0535648792515</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <f>F9</f>
         <v>285.07125449016206</v>
@@ -3762,15 +3764,15 @@
       <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -3787,7 +3789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
@@ -3804,7 +3806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -3844,7 +3846,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -3866,7 +3868,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -3888,7 +3890,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -3910,7 +3912,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -3932,7 +3934,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -3976,7 +3978,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -3998,7 +4000,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -4020,7 +4022,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -4042,7 +4044,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -4064,7 +4066,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -4086,7 +4088,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -4108,7 +4110,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -4130,7 +4132,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -4152,7 +4154,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -4174,7 +4176,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -4196,7 +4198,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -4218,7 +4220,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -4240,7 +4242,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -4284,7 +4286,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -4303,7 +4305,7 @@
         <v>0.65340493239222042</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -4322,7 +4324,7 @@
         <v>0.65478040208373045</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -4341,7 +4343,7 @@
         <v>0.48306046808804126</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -4360,7 +4362,7 @@
         <v>0.65556898779971107</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -4382,7 +4384,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -4404,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -4426,7 +4428,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -4448,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -4470,7 +4472,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>31</v>
       </c>

</xml_diff>